<commit_message>
Add Anenome species to connecticut ant-dispersed plant list.
</commit_message>
<xml_diff>
--- a/Data/ma thesis data Myrmecochores of southern new england.xlsx
+++ b/Data/ma thesis data Myrmecochores of southern new england.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailwsu-my.sharepoint.com/personal/robert_e_clark_wsu_edu/Documents/Henry-Buck-Trail-Experiment/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R Projects\Henry-Buck-Trail-Experiment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D5EDE74-8D87-4C98-A7FD-561431482B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270EB74B-20E4-46CD-925F-257E1BFA5074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="705" windowWidth="17258" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,24 @@
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={42A85D1D-ABC3-4164-A5C8-A6678AB1298E}</author>
+  </authors>
+  <commentList>
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{42A85D1D-ABC3-4164-A5C8-A6678AB1298E}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Now a subspecies of Viola pubescens</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -361,7 +379,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,6 +394,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -416,6 +440,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Robert Clark" id="{4810AF41-74A7-47B0-A571-9749D1149873}" userId="dd7e05961dafe2a8" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -737,28 +767,36 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A13" dT="2021-12-08T19:38:14.58" personId="{4810AF41-74A7-47B0-A571-9749D1149873}" id="{42A85D1D-ABC3-4164-A5C8-A6678AB1298E}">
+    <text>Now a subspecies of Viola pubescens</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="29.88671875" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" customWidth="1"/>
+    <col min="1" max="2" width="29.86328125" customWidth="1"/>
+    <col min="3" max="3" width="44.86328125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="9.86328125" customWidth="1"/>
+    <col min="6" max="6" width="22.53125" customWidth="1"/>
+    <col min="7" max="7" width="16.53125" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="21.88671875" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="21.86328125" customWidth="1"/>
+    <col min="11" max="11" width="14.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -775,7 +813,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -807,7 +845,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -830,7 +868,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -847,7 +885,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -861,7 +899,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -869,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -886,7 +924,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -903,7 +941,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -917,7 +955,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -925,7 +963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -933,7 +971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -941,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -949,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -957,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -968,7 +1006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -982,7 +1020,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -990,7 +1028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1007,7 +1045,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1024,7 +1062,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -1038,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1052,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1063,7 +1101,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1077,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1091,22 +1129,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1114,7 +1152,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1125,7 +1163,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -1136,7 +1174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -1147,7 +1185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -1158,7 +1196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -1169,7 +1207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -1183,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>64</v>
       </c>
@@ -1194,12 +1232,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -1216,7 +1254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -1233,7 +1271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -1244,7 +1282,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>74</v>
       </c>
@@ -1261,7 +1299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>77</v>
       </c>
@@ -1278,7 +1316,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>80</v>
       </c>
@@ -1295,7 +1333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>83</v>
       </c>
@@ -1312,7 +1350,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -1329,7 +1367,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -1346,7 +1384,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -1366,7 +1404,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>93</v>
       </c>
@@ -1383,7 +1421,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>99</v>
       </c>
@@ -1396,6 +1434,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1405,7 +1444,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1417,7 +1456,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>